<commit_message>
updating Please Select Logic
</commit_message>
<xml_diff>
--- a/feedback_forms/testing_versions/oil_and_gas_operator_feedback_v070_compled_01.xlsx
+++ b/feedback_forms/testing_versions/oil_and_gas_operator_feedback_v070_compled_01.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb-my.sharepoint.com/personal/tony_held_arb_ca_gov/Documents/code/pycharm/feedback_portal/feedback_forms/testing_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{597B706A-FF33-4B17-A9CF-CF195352088D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B41E77A-2466-43D5-99FB-9A26A7D73E32}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{597B706A-FF33-4B17-A9CF-CF195352088D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{300177FA-ED24-4E42-965A-2035EEE894A2}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kjlmzu+Q6SFTogsx4Qi52aIyd+8jmZeb0EwHe9aMejtDjbzj4NdjjdeuWfsACHLWYXh5VX6pk8UjIKzypXD1rg==" workbookSaltValue="GL9SubWR9+G9ealuHbyojg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4547" yWindow="2500" windowWidth="19200" windowHeight="11093" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
+    <workbookView xWindow="8227" yWindow="1267" windowWidth="17226" windowHeight="13020" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="5" r:id="rId1"/>
@@ -3022,8 +3022,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AG76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.5"/>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="C34" s="34"/>
       <c r="D34" s="61">
-        <v>45791</v>
+        <v>45791.599305555559</v>
       </c>
       <c r="E34" s="44"/>
       <c r="F34" s="44"/>
@@ -4292,7 +4292,7 @@
       </c>
       <c r="C55" s="44"/>
       <c r="D55" s="64">
-        <v>45294</v>
+        <v>45294.25</v>
       </c>
       <c r="E55" s="38"/>
       <c r="F55" s="44"/>
@@ -7371,6 +7371,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -7605,17 +7616,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
   <ds:schemaRefs>
@@ -7625,6 +7625,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368BC477-8FFD-4C56-8224-F3CCFEFBFA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533C6BB5-3BBA-46E5-A63A-38A55F0F20F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7641,15 +7652,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368BC477-8FFD-4C56-8224-F3CCFEFBFA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>